<commit_message>
Manual notes till feb 14th
</commit_message>
<xml_diff>
--- a/Test Case Template  - Adactin Registration.xlsx
+++ b/Test Case Template  - Adactin Registration.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\009LiveTech\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41831132-1AA9-4EEB-85F5-09ED1A5B5D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,15 +21,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -446,7 +443,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -547,7 +544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -557,10 +554,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -869,37 +864,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView topLeftCell="A34" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="53" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="93.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="93.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -907,7 +902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -918,7 +913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -926,7 +921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -934,7 +929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -942,7 +937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -977,7 +972,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="70.150000000000006" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="70.2" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -1006,7 +1001,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1020,7 +1015,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1034,7 +1029,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1048,7 +1043,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1059,7 +1054,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="H12" s="1" t="s">
         <v>46</v>
       </c>
@@ -1090,7 +1085,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1104,7 +1099,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1118,7 +1113,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1169,7 +1164,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1183,7 +1178,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1197,7 +1192,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E22" s="1" t="s">
         <v>28</v>
       </c>
@@ -1248,7 +1243,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1262,7 +1257,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1276,7 +1271,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1324,7 +1319,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E32" s="1" t="s">
         <v>25</v>
       </c>
@@ -1335,7 +1330,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="46.9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
       <c r="E33" s="1" t="s">
         <v>27</v>
       </c>
@@ -1346,7 +1341,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="70.150000000000006" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" ht="70.2" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -1369,7 +1364,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E36" s="1" t="s">
         <v>25</v>
       </c>
@@ -1380,7 +1375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E37" s="1" t="s">
         <v>27</v>
       </c>
@@ -1394,7 +1389,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="46.9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
       <c r="E38" s="1" t="s">
         <v>28</v>
       </c>
@@ -1428,7 +1423,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E41" s="1" t="s">
         <v>25</v>
       </c>
@@ -1439,7 +1434,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="23.45" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E42" s="1" t="s">
         <v>27</v>
       </c>
@@ -1453,7 +1448,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="46.9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
       <c r="E43" s="1" t="s">
         <v>28</v>
       </c>
@@ -1490,7 +1485,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E46" s="1" t="s">
         <v>25</v>
       </c>
@@ -1504,7 +1499,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E47" s="1" t="s">
         <v>27</v>
       </c>
@@ -1518,7 +1513,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E48" s="1" t="s">
         <v>28</v>
       </c>
@@ -1532,7 +1527,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E49" s="1" t="s">
         <v>29</v>
       </c>
@@ -1543,7 +1538,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="5:8" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:8" ht="46.8" x14ac:dyDescent="0.45">
       <c r="H50" s="5" t="s">
         <v>70</v>
       </c>
@@ -1555,29 +1550,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="73.42578125" customWidth="1"/>
-    <col min="7" max="7" width="37.85546875" customWidth="1"/>
-    <col min="8" max="8" width="77.42578125" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45.88671875" customWidth="1"/>
+    <col min="2" max="2" width="53.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="73.44140625" customWidth="1"/>
+    <col min="7" max="7" width="37.88671875" customWidth="1"/>
+    <col min="8" max="8" width="77.44140625" customWidth="1"/>
+    <col min="9" max="9" width="24.44140625" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1594,7 +1589,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1613,7 +1608,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1630,7 +1625,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1647,7 +1642,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1664,7 +1659,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1699,11 +1694,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A7" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>100</v>
       </c>
       <c r="C7" t="s">
@@ -1725,7 +1720,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1739,7 +1734,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1751,7 +1746,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1759,122 +1754,122 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E11" s="7" t="s">
+    <row r="11" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E12" s="7" t="s">
+    <row r="12" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E13" s="7" t="s">
+    <row r="13" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E13" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E14" s="7" t="s">
+    <row r="14" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E14" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E15" s="7" t="s">
+    <row r="15" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E15" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E16" s="7" t="s">
+    <row r="16" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E16" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E17" s="7" t="s">
+    <row r="17" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E17" s="1" t="s">
         <v>96</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E18" s="7" t="s">
+    <row r="18" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E18" s="1" t="s">
         <v>97</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="H19" s="7" t="s">
+    <row r="19" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="H19" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:8" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="A20" s="9" t="s">
         <v>98</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="7" t="s">
         <v>99</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -1890,7 +1885,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E21" s="1" t="s">
         <v>25</v>
       </c>
@@ -1904,7 +1899,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1916,7 +1911,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -1924,86 +1919,86 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E24" s="7" t="s">
+    <row r="24" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H24" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E25" s="7" t="s">
+    <row r="25" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E25" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E26" s="7" t="s">
+    <row r="26" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E26" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E27" s="7" t="s">
+    <row r="27" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E27" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H27" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E28" s="7" t="s">
+    <row r="28" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E28" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H28" s="7" t="s">
+      <c r="H28" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E29" s="7" t="s">
+    <row r="29" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E29" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="H29" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="E30" s="7" t="s">
+    <row r="30" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="E30" s="1" t="s">
         <v>96</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -2013,18 +2008,18 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F31" s="1"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:8" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A32" s="11" t="s">
+    <row r="32" spans="1:8" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="A32" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="7" t="s">
         <v>103</v>
       </c>
       <c r="E32" s="1" t="s">
@@ -2040,7 +2035,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E33" s="1" t="s">
         <v>25</v>
       </c>
@@ -2054,7 +2049,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E34" s="1" t="s">
         <v>27</v>
       </c>
@@ -2066,7 +2061,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -2074,86 +2069,86 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E36" s="7" t="s">
+    <row r="36" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="G36" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H36" s="7" t="s">
+      <c r="H36" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E37" s="7" t="s">
+    <row r="37" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E37" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="G37" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H37" s="7" t="s">
+      <c r="H37" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E38" s="7" t="s">
+    <row r="38" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E38" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="G38" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H38" s="7" t="s">
+      <c r="H38" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E39" s="7" t="s">
+    <row r="39" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E39" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="G39" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H39" s="7" t="s">
+      <c r="H39" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E40" s="7" t="s">
+    <row r="40" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E40" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H40" s="7" t="s">
+      <c r="H40" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E41" s="7" t="s">
+    <row r="41" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E41" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H41" s="7" t="s">
+      <c r="H41" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="E42" s="7" t="s">
+    <row r="42" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="E42" s="1" t="s">
         <v>96</v>
       </c>
       <c r="F42" s="1" t="s">
@@ -2163,14 +2158,14 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A44" s="11" t="s">
+    <row r="44" spans="1:8" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="A44" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="7" t="s">
         <v>107</v>
       </c>
       <c r="E44" s="1" t="s">
@@ -2186,7 +2181,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E45" s="1" t="s">
         <v>25</v>
       </c>
@@ -2200,7 +2195,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E46" s="1" t="s">
         <v>27</v>
       </c>
@@ -2212,7 +2207,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -2220,86 +2215,86 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E48" s="7" t="s">
+    <row r="48" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E48" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F48" s="7" t="s">
+      <c r="F48" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G48" s="7" t="s">
+      <c r="G48" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H48" s="7" t="s">
+      <c r="H48" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E49" s="7" t="s">
+    <row r="49" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E49" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G49" s="7" t="s">
+      <c r="G49" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H49" s="7" t="s">
+      <c r="H49" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E50" s="7" t="s">
+    <row r="50" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E50" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G50" s="7" t="s">
+      <c r="G50" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H50" s="7" t="s">
+      <c r="H50" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E51" s="7" t="s">
+    <row r="51" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E51" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G51" s="9" t="s">
+      <c r="G51" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H51" s="7" t="s">
+      <c r="H51" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E52" s="7" t="s">
+    <row r="52" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E52" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H52" s="7" t="s">
+      <c r="H52" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E53" s="7" t="s">
+    <row r="53" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E53" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H53" s="7" t="s">
+      <c r="H53" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="E54" s="7" t="s">
+    <row r="54" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="E54" s="1" t="s">
         <v>96</v>
       </c>
       <c r="F54" s="1" t="s">
@@ -2309,15 +2304,15 @@
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A56" s="11" t="s">
+    <row r="55" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="A56" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="7" t="s">
         <v>107</v>
       </c>
       <c r="E56" s="1" t="s">
@@ -2333,7 +2328,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E57" s="1" t="s">
         <v>25</v>
       </c>
@@ -2347,7 +2342,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E58" s="1" t="s">
         <v>27</v>
       </c>
@@ -2359,7 +2354,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -2367,86 +2362,86 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E60" s="7" t="s">
+    <row r="60" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E60" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F60" s="7" t="s">
+      <c r="F60" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G60" s="7" t="s">
+      <c r="G60" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H60" s="7" t="s">
+      <c r="H60" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E61" s="7" t="s">
+    <row r="61" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E61" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G61" s="7" t="s">
+      <c r="G61" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H61" s="7" t="s">
+      <c r="H61" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E62" s="7" t="s">
+    <row r="62" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E62" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G62" s="7" t="s">
+      <c r="G62" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H62" s="7" t="s">
+      <c r="H62" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E63" s="7" t="s">
+    <row r="63" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E63" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G63" s="9" t="s">
+      <c r="G63" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H63" s="7" t="s">
+      <c r="H63" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E64" s="7" t="s">
+    <row r="64" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E64" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H64" s="7" t="s">
+      <c r="H64" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E65" s="7" t="s">
+    <row r="65" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E65" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H65" s="7" t="s">
+      <c r="H65" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="E66" s="7" t="s">
+    <row r="66" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="E66" s="1" t="s">
         <v>96</v>
       </c>
       <c r="F66" s="1" t="s">
@@ -2456,19 +2451,19 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E67" s="7"/>
+    <row r="67" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="H67" s="5"/>
     </row>
-    <row r="68" spans="1:8" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A68" s="11" t="s">
+    <row r="68" spans="1:8" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="A68" s="9" t="s">
         <v>116</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C68" s="10" t="s">
+      <c r="C68" s="7" t="s">
         <v>118</v>
       </c>
       <c r="E68" s="1" t="s">
@@ -2484,7 +2479,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E69" s="1" t="s">
         <v>25</v>
       </c>
@@ -2498,7 +2493,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E70" s="1" t="s">
         <v>27</v>
       </c>
@@ -2510,7 +2505,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -2518,86 +2513,86 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E72" s="7" t="s">
+    <row r="72" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E72" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F72" s="7" t="s">
+      <c r="F72" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G72" s="7" t="s">
+      <c r="G72" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H72" s="7" t="s">
+      <c r="H72" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E73" s="7" t="s">
+    <row r="73" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E73" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G73" s="7" t="s">
+      <c r="G73" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H73" s="7" t="s">
+      <c r="H73" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E74" s="7" t="s">
+    <row r="74" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E74" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G74" s="7" t="s">
+      <c r="G74" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H74" s="7" t="s">
+      <c r="H74" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E75" s="7" t="s">
+    <row r="75" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E75" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G75" s="7" t="s">
+      <c r="G75" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H75" s="7" t="s">
+      <c r="H75" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E76" s="7" t="s">
+    <row r="76" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E76" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H76" s="7" t="s">
+      <c r="H76" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E77" s="7" t="s">
+    <row r="77" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E77" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H77" s="7" t="s">
+      <c r="H77" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="E78" s="7" t="s">
+    <row r="78" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="E78" s="1" t="s">
         <v>96</v>
       </c>
       <c r="F78" s="1" t="s">
@@ -2607,14 +2602,14 @@
         <v>120</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A80" s="11" t="s">
+    <row r="80" spans="1:8" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="A80" s="9" t="s">
         <v>121</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C80" s="10" t="s">
+      <c r="C80" s="7" t="s">
         <v>122</v>
       </c>
       <c r="E80" s="1" t="s">
@@ -2630,7 +2625,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E81" s="1" t="s">
         <v>25</v>
       </c>
@@ -2644,7 +2639,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E82" s="1" t="s">
         <v>27</v>
       </c>
@@ -2656,7 +2651,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
@@ -2664,89 +2659,89 @@
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E84" s="7" t="s">
+    <row r="84" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E84" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F84" s="8" t="s">
+      <c r="F84" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G84" s="7" t="s">
+      <c r="G84" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H84" s="7" t="s">
+      <c r="H84" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E85" s="7" t="s">
+    <row r="85" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E85" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F85" s="7" t="s">
+      <c r="F85" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G85" s="7" t="s">
+      <c r="G85" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H85" s="7" t="s">
+      <c r="H85" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E86" s="7" t="s">
+    <row r="86" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E86" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G86" s="7" t="s">
+      <c r="G86" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H86" s="7" t="s">
+      <c r="H86" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E87" s="7" t="s">
+    <row r="87" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E87" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G87" s="7" t="s">
+      <c r="G87" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H87" s="7" t="s">
+      <c r="H87" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E88" s="7" t="s">
+    <row r="88" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E88" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G88" s="9" t="s">
+      <c r="G88" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H88" s="7" t="s">
+      <c r="H88" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E89" s="7" t="s">
+    <row r="89" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E89" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H89" s="7" t="s">
+      <c r="H89" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="E90" s="7" t="s">
+    <row r="90" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="E90" s="1" t="s">
         <v>96</v>
       </c>
       <c r="F90" s="1" t="s">
@@ -2756,17 +2751,17 @@
         <v>124</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="H91" s="7"/>
-    </row>
-    <row r="92" spans="1:8" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A92" s="11" t="s">
+    <row r="91" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="H91" s="1"/>
+    </row>
+    <row r="92" spans="1:8" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="A92" s="9" t="s">
         <v>125</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C92" s="10" t="s">
+      <c r="C92" s="7" t="s">
         <v>127</v>
       </c>
       <c r="E92" s="1" t="s">
@@ -2782,7 +2777,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E93" s="1" t="s">
         <v>25</v>
       </c>
@@ -2796,7 +2791,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E94" s="1" t="s">
         <v>27</v>
       </c>
@@ -2808,7 +2803,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
@@ -2816,100 +2811,100 @@
         <v>74</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E96" s="7" t="s">
+    <row r="96" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E96" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F96" s="8" t="s">
+      <c r="F96" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G96" s="7" t="s">
+      <c r="G96" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H96" s="7" t="s">
+      <c r="H96" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E97" s="7" t="s">
+    <row r="97" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E97" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F97" s="7" t="s">
+      <c r="F97" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G97" s="7" t="s">
+      <c r="G97" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H97" s="7" t="s">
+      <c r="H97" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E98" s="7" t="s">
+    <row r="98" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E98" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G98" s="7" t="s">
+      <c r="G98" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H98" s="7" t="s">
+      <c r="H98" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E99" s="7" t="s">
+    <row r="99" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E99" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G99" s="7" t="s">
+      <c r="G99" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H99" s="7" t="s">
+      <c r="H99" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E100" s="7" t="s">
+    <row r="100" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E100" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G100" s="9" t="s">
+      <c r="G100" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H100" s="7" t="s">
+      <c r="H100" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E101" s="7" t="s">
+    <row r="101" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E101" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H101" s="7" t="s">
+      <c r="H101" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E102" s="7" t="s">
+    <row r="102" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E102" s="1" t="s">
         <v>96</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H102" s="7" t="s">
+      <c r="H102" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="E103" s="7" t="s">
+    <row r="103" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="E103" s="1" t="s">
         <v>97</v>
       </c>
       <c r="F103" s="1" t="s">
@@ -2919,17 +2914,17 @@
         <v>128</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="H104" s="7"/>
-    </row>
-    <row r="105" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A105" s="11" t="s">
+    <row r="104" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="H104" s="1"/>
+    </row>
+    <row r="105" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A105" s="9" t="s">
         <v>129</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C105" s="10" t="s">
+      <c r="C105" s="7" t="s">
         <v>131</v>
       </c>
       <c r="E105" s="1" t="s">
@@ -2945,7 +2940,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E106" s="1" t="s">
         <v>25</v>
       </c>
@@ -2959,7 +2954,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E107" s="1" t="s">
         <v>27</v>
       </c>
@@ -2971,7 +2966,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
@@ -2979,8 +2974,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="116.25" x14ac:dyDescent="0.35">
-      <c r="E109" s="7" t="s">
+    <row r="109" spans="1:8" ht="117" x14ac:dyDescent="0.45">
+      <c r="E109" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F109" s="1" t="s">
@@ -2992,13 +2987,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G15" r:id="rId1"/>
-    <hyperlink ref="G27" r:id="rId2"/>
-    <hyperlink ref="G39" r:id="rId3"/>
-    <hyperlink ref="G51" r:id="rId4"/>
-    <hyperlink ref="G63" r:id="rId5"/>
-    <hyperlink ref="G88" r:id="rId6"/>
-    <hyperlink ref="G100" r:id="rId7"/>
+    <hyperlink ref="G15" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G27" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="G39" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="G51" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="G63" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="G88" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="G100" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>

<commit_message>
Java Season 1 Notes
</commit_message>
<xml_diff>
--- a/Test Case Template  - Adactin Registration.xlsx
+++ b/Test Case Template  - Adactin Registration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\009LiveTech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41831132-1AA9-4EEB-85F5-09ED1A5B5D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE29B13-6440-46D5-AF75-2E56BA806E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="135">
   <si>
     <t>Project Name</t>
   </si>
@@ -438,6 +438,12 @@
   <si>
     <t>Error should display below text 
 " Username is Empty""Password is Empty""Confirm Password is Empty""Full Name is Empty""Email Address is Empty""Captcha is Empty""You must agree to Terms and Conditions"</t>
+  </si>
+  <si>
+    <t>Riyaz</t>
+  </si>
+  <si>
+    <t>Venkat Ramana</t>
   </si>
 </sst>
 </file>
@@ -544,7 +550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -557,6 +563,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1553,8 +1560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1604,7 +1611,9 @@
       <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
@@ -1621,7 +1630,9 @@
       <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="10">
+        <v>45341</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
@@ -1638,7 +1649,9 @@
       <c r="H4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
@@ -1655,7 +1668,9 @@
       <c r="H5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="10">
+        <v>45342</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>

</xml_diff>